<commit_message>
Story DB: - Added column 'instructions' to table 'chapters'. - Added columns 'instructions', 'feedback_right', 'feedback_wrong', 'audiopath_right' and 'audiopath_wrong' to the tables 'nfc', 'qr', 'gps' and 'spell'. - Added columns 'feedback_right', 'feedback_wrong', 'audiopath_right' and 'audiopath_wrong' to the table 'quiz'. - All changes done with descriptions are on file /documentation/DB Story design.xlsx.
Story JSON:
- Necessary keys were added in chapters and interactions to meet new DB scheme.
- For columns 'audiopath_right' and 'audiopath_wrong', the key in the JSON are 'feedbackurl_right' and 'feedbackurl_wrong' respectively. It should work as the video urls on chapter.
</commit_message>
<xml_diff>
--- a/documentation/DB Story design.xlsx
+++ b/documentation/DB Story design.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanCamilo\Documents\Oulu\SP\story\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7740"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="DB Story" sheetId="1" r:id="rId3"/>
+    <sheet name="DB Story" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="129">
   <si>
     <t>Table Authors</t>
   </si>
@@ -365,28 +373,64 @@
   </si>
   <si>
     <t>Version of the database</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>Question / Instructions for the interaction</t>
+  </si>
+  <si>
+    <t>feedback_right</t>
+  </si>
+  <si>
+    <t>feedback_wrong</t>
+  </si>
+  <si>
+    <t>audiopath_right</t>
+  </si>
+  <si>
+    <t>audiopath_wrong</t>
+  </si>
+  <si>
+    <t>Instructions to do the interaction</t>
+  </si>
+  <si>
+    <t>Text feedback if the interaction is done correctly</t>
+  </si>
+  <si>
+    <t>Text feedback if the interaction is done wrongly</t>
+  </si>
+  <si>
+    <t>Audio path of feedback if the interaction is done wrongly</t>
+  </si>
+  <si>
+    <t>Audio path of feedback if the interaction is done correctly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -399,6 +443,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -411,6 +456,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -421,6 +467,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -429,6 +476,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -439,6 +487,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -449,6 +498,7 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -457,6 +507,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -465,6 +516,7 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -475,6 +527,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -483,6 +536,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -493,6 +547,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -505,79 +560,424 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+  <cellXfs count="33">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="20.57"/>
-    <col customWidth="1" max="5" min="5" width="61.0"/>
-    <col customWidth="1" max="6" min="6" width="58.57"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="61" customWidth="1"/>
+    <col min="6" max="6" width="58.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -588,14 +988,14 @@
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -612,7 +1012,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -629,7 +1029,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -646,7 +1046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -663,7 +1063,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -680,7 +1080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
@@ -697,13 +1097,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
@@ -714,14 +1114,14 @@
       <c r="E11" s="4"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="14"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="7" t="s">
         <v>4</v>
       </c>
@@ -735,7 +1135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
         <v>31</v>
       </c>
@@ -749,7 +1149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="7" t="s">
         <v>14</v>
       </c>
@@ -761,7 +1161,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="7" t="s">
         <v>34</v>
       </c>
@@ -775,7 +1175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="10" t="s">
         <v>9</v>
       </c>
@@ -789,7 +1189,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="3" t="s">
         <v>38</v>
       </c>
@@ -797,11 +1197,11 @@
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20">
+    <row r="20" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="14"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21">
+    <row r="21" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="7" t="s">
         <v>4</v>
       </c>
@@ -815,7 +1215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="7" t="s">
         <v>39</v>
       </c>
@@ -829,7 +1229,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="7" t="s">
         <v>31</v>
       </c>
@@ -843,7 +1243,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C24" s="7" t="s">
         <v>43</v>
       </c>
@@ -855,7 +1255,7 @@
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="25">
+    <row r="25" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C25" s="7" t="s">
         <v>14</v>
       </c>
@@ -867,7 +1267,7 @@
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26">
+    <row r="26" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C26" s="7" t="s">
         <v>46</v>
       </c>
@@ -881,7 +1281,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C27" s="7" t="s">
         <v>48</v>
       </c>
@@ -895,7 +1295,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C28" s="7" t="s">
         <v>50</v>
       </c>
@@ -909,7 +1309,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="7" t="s">
         <v>52</v>
       </c>
@@ -923,7 +1323,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C30" s="7" t="s">
         <v>54</v>
       </c>
@@ -937,370 +1337,398 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31">
-      <c r="C31" s="7"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32">
-      <c r="C32" s="10" t="s">
+    <row r="31" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C31" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C32" s="7"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C33" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="12"/>
-    </row>
-    <row r="34">
-      <c r="C34" s="3" t="s">
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="12"/>
+    </row>
+    <row r="35" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C35" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35">
-      <c r="C35" s="14"/>
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36">
-      <c r="C36" s="7" t="s">
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C36" s="14"/>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C37" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F37" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37">
-      <c r="C37" s="7" t="s">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C38" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38">
-      <c r="C38" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="H38" s="1"/>
     </row>
-    <row r="39">
+    <row r="39" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C39" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H39" s="1"/>
     </row>
-    <row r="40">
+    <row r="40" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C40" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H40" s="1"/>
     </row>
-    <row r="41">
+    <row r="41" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C41" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H41" s="1"/>
     </row>
-    <row r="42">
+    <row r="42" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C42" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H42" s="1"/>
     </row>
-    <row r="43">
+    <row r="43" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C43" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C44" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F44" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44">
-      <c r="C44" s="14"/>
-      <c r="F44" s="8"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45">
-      <c r="C45" s="10" t="s">
+    <row r="45" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C45" s="14"/>
+      <c r="F45" s="8"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C46" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="16"/>
-      <c r="H45" s="1"/>
-    </row>
-    <row r="46">
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="16"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47">
-      <c r="C47" s="3" t="s">
+    <row r="47" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C48" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="5"/>
-      <c r="H47" s="1"/>
-    </row>
-    <row r="48">
-      <c r="C48" s="7"/>
-      <c r="F48" s="8"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="5"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49">
-      <c r="C49" s="7" t="s">
+    <row r="49" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C49" s="7"/>
+      <c r="F49" s="8"/>
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C50" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F50" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="1"/>
-    </row>
-    <row r="50">
-      <c r="C50" s="7" t="s">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C51" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F51" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="1"/>
-    </row>
-    <row r="51">
-      <c r="C51" s="7" t="s">
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C52" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="1" t="s">
+      <c r="D52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F51" s="9" t="s">
+      <c r="F52" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H51" s="1"/>
-    </row>
-    <row r="52">
-      <c r="C52" s="10" t="s">
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C53" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D52" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="11" t="s">
+      <c r="D53" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F53" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="H52" s="1"/>
-    </row>
-    <row r="53">
       <c r="H53" s="1"/>
     </row>
-    <row r="54">
-      <c r="C54" s="3" t="s">
+    <row r="54" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C55" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="5"/>
-    </row>
-    <row r="55">
-      <c r="C55" s="14"/>
-      <c r="F55" s="8"/>
-    </row>
-    <row r="56">
-      <c r="C56" s="7" t="s">
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="22"/>
+    </row>
+    <row r="56" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C56" s="23"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="24"/>
+    </row>
+    <row r="57" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C57" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F57" s="26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57">
-      <c r="C57" s="7" t="s">
+    <row r="58" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C58" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F58" s="26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58">
-      <c r="C58" s="10" t="s">
+    <row r="59" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C59" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="D58" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E58" s="11" t="s">
+      <c r="D59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F58" s="16"/>
-    </row>
-    <row r="60">
-      <c r="C60" s="3" t="s">
+      <c r="F59" s="26"/>
+    </row>
+    <row r="60" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C60" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F60" s="26"/>
+    </row>
+    <row r="61" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C61" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F61" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C62" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F62" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C63" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C64" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F64" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C66" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="5"/>
-    </row>
-    <row r="61">
-      <c r="C61" s="14"/>
-      <c r="F61" s="8"/>
-    </row>
-    <row r="62">
-      <c r="C62" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="C63" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="C64" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F64" s="16"/>
-    </row>
-    <row r="65">
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-    </row>
-    <row r="66">
-      <c r="C66" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="5"/>
-    </row>
-    <row r="67">
-      <c r="C67" s="14"/>
-      <c r="F67" s="8"/>
-    </row>
-    <row r="68">
-      <c r="C68" s="7" t="s">
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="22"/>
+    </row>
+    <row r="67" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C67" s="23"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="24"/>
+    </row>
+    <row r="68" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C68" s="25" t="s">
         <v>4</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -1309,13 +1737,13 @@
       <c r="E68" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F68" s="9" t="s">
+      <c r="F68" s="26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="69">
-      <c r="C69" s="7" t="s">
-        <v>68</v>
+    <row r="69" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C69" s="25" t="s">
+        <v>65</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>10</v>
@@ -1323,206 +1751,246 @@
       <c r="E69" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F69" s="26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="70">
-      <c r="C70" s="7" t="s">
+    <row r="70" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C70" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F70" s="24"/>
+    </row>
+    <row r="71" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C71" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F71" s="26"/>
+    </row>
+    <row r="72" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C72" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F72" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C73" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F73" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C74" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F74" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C75" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D75" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F75" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+    </row>
+    <row r="77" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C77" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="22"/>
+    </row>
+    <row r="78" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C78" s="23"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="24"/>
+    </row>
+    <row r="79" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C79" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F79" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C80" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F80" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C81" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F70" s="8"/>
-    </row>
-    <row r="71">
-      <c r="C71" s="10" t="s">
+      <c r="F81" s="24"/>
+    </row>
+    <row r="82" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C82" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="D71" s="11" t="s">
+      <c r="D82" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="11" t="s">
+      <c r="E82" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F71" s="16"/>
-    </row>
-    <row r="73">
-      <c r="C73" s="3" t="s">
+      <c r="F82" s="24"/>
+    </row>
+    <row r="83" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C83" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F83" s="26"/>
+    </row>
+    <row r="84" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C84" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E84" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F84" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C85" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F85" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C86" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E86" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F86" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C87" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D87" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E87" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F87" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C89" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="5"/>
-    </row>
-    <row r="74">
-      <c r="C74" s="14"/>
-      <c r="F74" s="8"/>
-    </row>
-    <row r="75">
-      <c r="C75" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="C76" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="C77" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="F77" s="16"/>
-    </row>
-    <row r="79">
-      <c r="C79" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="5"/>
-    </row>
-    <row r="80">
-      <c r="C80" s="14"/>
-      <c r="F80" s="8"/>
-    </row>
-    <row r="81">
-      <c r="C81" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="C82" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="C83" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F83" s="8"/>
-    </row>
-    <row r="84">
-      <c r="C84" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F84" s="8"/>
-    </row>
-    <row r="85">
-      <c r="C85" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F85" s="8"/>
-    </row>
-    <row r="86">
-      <c r="C86" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F86" s="9"/>
-    </row>
-    <row r="87">
-      <c r="C87" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="F87" s="12"/>
-    </row>
-    <row r="88">
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-    </row>
-    <row r="89">
-      <c r="C89" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="5"/>
-    </row>
-    <row r="90">
-      <c r="C90" s="14"/>
-      <c r="F90" s="8"/>
-    </row>
-    <row r="91">
-      <c r="C91" s="7" t="s">
+      <c r="D89" s="21"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="22"/>
+    </row>
+    <row r="90" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C90" s="23"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="24"/>
+    </row>
+    <row r="91" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C91" s="25" t="s">
         <v>4</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -1531,47 +1999,331 @@
       <c r="E91" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F91" s="9" t="s">
+      <c r="F91" s="26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="92">
-      <c r="C92" s="10" t="s">
+    <row r="92" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C92" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F92" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C93" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F93" s="24"/>
+    </row>
+    <row r="94" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C94" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E94" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F94" s="26"/>
+    </row>
+    <row r="95" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C95" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E95" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F95" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C96" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E96" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F96" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C97" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E97" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F97" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C98" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D98" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E98" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F98" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C100" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D100" s="21"/>
+      <c r="E100" s="21"/>
+      <c r="F100" s="22"/>
+    </row>
+    <row r="101" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C101" s="23"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="24"/>
+    </row>
+    <row r="102" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C102" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F102" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C103" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F103" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C104" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F104" s="24"/>
+    </row>
+    <row r="105" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C105" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F105" s="24"/>
+    </row>
+    <row r="106" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C106" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F106" s="24"/>
+    </row>
+    <row r="107" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C107" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F107" s="26"/>
+    </row>
+    <row r="108" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C108" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F108" s="26"/>
+    </row>
+    <row r="109" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C109" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D109" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E109" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F109" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C110" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D110" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F110" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C111" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D111" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E111" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F111" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C112" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D112" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F112" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+    </row>
+    <row r="114" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C114" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="5"/>
+    </row>
+    <row r="115" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C115" s="14"/>
+      <c r="F115" s="8"/>
+    </row>
+    <row r="116" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C116" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C117" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D92" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E92" s="11" t="s">
+      <c r="D117" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E117" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="F92" s="16"/>
-    </row>
-    <row r="93">
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-    </row>
-    <row r="94">
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-    </row>
-    <row r="95">
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-    </row>
-    <row r="96">
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-    </row>
-    <row r="97">
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-    </row>
-    <row r="98">
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
+      <c r="F117" s="16"/>
+    </row>
+    <row r="118" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+    </row>
+    <row r="119" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+    </row>
+    <row r="120" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+    </row>
+    <row r="121" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+    </row>
+    <row r="122" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+    </row>
+    <row r="123" spans="3:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>